<commit_message>
Fixed misspelled team name in the bracket.
</commit_message>
<xml_diff>
--- a/2015/NCAA.xlsx
+++ b/2015/NCAA.xlsx
@@ -153,9 +153,6 @@
     <t>9 Louisiana St.</t>
   </si>
   <si>
-    <t>5 Northen Iowa</t>
-  </si>
-  <si>
     <t>12 Wyoming</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>15 Texas Southern</t>
+  </si>
+  <si>
+    <t>5 Northern Iowa</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -397,21 +412,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -773,823 +773,775 @@
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="8">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="9"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="9"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="9"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="9"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="9"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="9"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="9"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="9"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="9"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="9"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="9"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="9"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="9"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="14"/>
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="14"/>
+    </row>
+    <row r="41" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="s">
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="14"/>
+    </row>
+    <row r="42" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="14"/>
+    </row>
+    <row r="43" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="14"/>
+    </row>
+    <row r="44" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="9"/>
-    </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13" t="s">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="14"/>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="14"/>
+    </row>
+    <row r="49" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="9"/>
-    </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="9"/>
-    </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="9"/>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="14"/>
+    </row>
+    <row r="52" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="9"/>
-    </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="14"/>
+    </row>
+    <row r="53" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="9"/>
-    </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="14"/>
+    </row>
+    <row r="54" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="9"/>
-    </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="15" t="s">
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="14"/>
+    </row>
+    <row r="55" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="9"/>
-    </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="14"/>
+    </row>
+    <row r="56" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="9"/>
-    </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="14"/>
+    </row>
+    <row r="57" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="9"/>
-    </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="15" t="s">
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="14"/>
+    </row>
+    <row r="58" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="9"/>
-    </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="14"/>
+    </row>
+    <row r="59" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="9"/>
-    </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="15" t="s">
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="14"/>
+    </row>
+    <row r="60" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="14"/>
+    </row>
+    <row r="61" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="9"/>
-    </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="9"/>
-    </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="15" t="s">
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="14"/>
+    </row>
+    <row r="62" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="9"/>
-    </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="14"/>
+    </row>
+    <row r="63" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="9"/>
-    </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="s">
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="14"/>
+    </row>
+    <row r="64" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="9"/>
-    </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="14"/>
+    </row>
+    <row r="65" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="9"/>
-    </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="10"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="15"/>
     </row>
     <row r="66" spans="1:8" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C46:C49"/>
     <mergeCell ref="D58:D65"/>
     <mergeCell ref="D2:D9"/>
     <mergeCell ref="H2:H65"/>
@@ -1606,6 +1558,54 @@
     <mergeCell ref="D34:D41"/>
     <mergeCell ref="D42:D49"/>
     <mergeCell ref="D50:D57"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>